<commit_message>
multiple equal poles 8 senza pida
</commit_message>
<xml_diff>
--- a/Benchmark_System/Multiple_Equals_poles4/Multiple Equal Poles4.xlsx
+++ b/Benchmark_System/Multiple_Equals_poles4/Multiple Equal Poles4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edoar\Documenti\git hub\PID_PIDA_Controller\Benchmark_System\Multiple_Equals_poles4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085154A0-4452-47DB-9BEA-19F70D3DE435}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72C32D6-D9C3-483B-A871-7ABD6E4199A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="1800" windowWidth="27000" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30135" yWindow="1575" windowWidth="27000" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reference traking" sheetId="1" r:id="rId1"/>
@@ -463,19 +463,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -732,6 +734,7 @@
         <v>3.10435069606784</v>
       </c>
     </row>
+    <row r="17" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -739,17 +742,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151A9C13-F3FF-454B-AAEA-BBA6AC050E96}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="B11:E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="5" customWidth="1"/>
     <col min="2" max="5" width="12.6640625" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="5"/>
+    <col min="6" max="6" width="8.88671875" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="5" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -934,6 +938,7 @@
         <v>15</v>
       </c>
     </row>
+    <row r="17" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>